<commit_message>
Update IL200_dyn_nl.xlsx and rerun casestudy
</commit_message>
<xml_diff>
--- a/ACTIVSg200/IL200_dyn_nl.xlsx
+++ b/ACTIVSg200/IL200_dyn_nl.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/work/turbinegov/ACTIVSg200/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9AF4EC1-C350-2B46-833E-8CBD1377B895}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE5535D-DCB8-684F-AD05-A34C3E246641}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1540" windowWidth="34560" windowHeight="19000" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="1540" windowWidth="34560" windowHeight="19000" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1917" uniqueCount="1009">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1918" uniqueCount="1010">
   <si>
     <t>idx</t>
   </si>
@@ -3062,6 +3062,9 @@
   </si>
   <si>
     <t>WTDS_6</t>
+  </si>
+  <si>
+    <t>CE</t>
   </si>
 </sst>
 </file>
@@ -3093,7 +3096,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -3116,13 +3119,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -12289,16 +12306,16 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:AB18"/>
+  <dimension ref="A1:AC18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q31" sqref="Q31"/>
+      <selection pane="bottomLeft" activeCell="AB12" sqref="AB12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -12383,8 +12400,11 @@
       <c r="AB1" s="1" t="s">
         <v>801</v>
       </c>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC1" s="2" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -12466,8 +12486,11 @@
       <c r="AB2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -12549,8 +12572,11 @@
       <c r="AB3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC3">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -12632,8 +12658,11 @@
       <c r="AB4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC4">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -12715,8 +12744,11 @@
       <c r="AB5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC5">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -12798,8 +12830,11 @@
       <c r="AB6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC6">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -12881,8 +12916,11 @@
       <c r="AB7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -12964,8 +13002,11 @@
       <c r="AB8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -13047,8 +13088,11 @@
       <c r="AB9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC9">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -13130,8 +13174,11 @@
       <c r="AB10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC10">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -13213,8 +13260,11 @@
       <c r="AB11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC11">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -13296,8 +13346,11 @@
       <c r="AB12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC12">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -13379,8 +13432,11 @@
       <c r="AB13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC13">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -13462,8 +13518,11 @@
       <c r="AB14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC14">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -13545,8 +13604,11 @@
       <c r="AB15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -13628,8 +13690,11 @@
       <c r="AB16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC16">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -13711,8 +13776,11 @@
       <c r="AB17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC17">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -13793,6 +13861,9 @@
       </c>
       <c r="AB18">
         <v>0</v>
+      </c>
+      <c r="AC18">
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
   </sheetData>
@@ -13804,9 +13875,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13884,7 +13955,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -13934,7 +14005,7 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -13984,7 +14055,7 @@
         <v>1</v>
       </c>
       <c r="H4">
-        <v>0.04</v>
+        <v>0.3</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -14034,7 +14105,7 @@
         <v>1</v>
       </c>
       <c r="H5">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="I5">
         <v>1</v>
@@ -14084,7 +14155,7 @@
         <v>1</v>
       </c>
       <c r="H6">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -14134,7 +14205,7 @@
         <v>1</v>
       </c>
       <c r="H7">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="I7">
         <v>1</v>
@@ -14184,7 +14255,7 @@
         <v>1</v>
       </c>
       <c r="H8">
-        <v>0.04</v>
+        <v>0.3</v>
       </c>
       <c r="I8">
         <v>1</v>
@@ -14234,7 +14305,7 @@
         <v>1</v>
       </c>
       <c r="H9">
-        <v>0.04</v>
+        <v>0.3</v>
       </c>
       <c r="I9">
         <v>1</v>
@@ -14284,7 +14355,7 @@
         <v>1</v>
       </c>
       <c r="H10">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="I10">
         <v>1</v>
@@ -14334,7 +14405,7 @@
         <v>1</v>
       </c>
       <c r="H11">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="I11">
         <v>1</v>
@@ -14384,7 +14455,7 @@
         <v>1</v>
       </c>
       <c r="H12">
-        <v>0.04</v>
+        <v>0.3</v>
       </c>
       <c r="I12">
         <v>1</v>
@@ -14434,7 +14505,7 @@
         <v>1</v>
       </c>
       <c r="H13">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="I13">
         <v>1</v>
@@ -14484,7 +14555,7 @@
         <v>1</v>
       </c>
       <c r="H14">
-        <v>0.04</v>
+        <v>0.3</v>
       </c>
       <c r="I14">
         <v>1</v>
@@ -14534,7 +14605,7 @@
         <v>1</v>
       </c>
       <c r="H15">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="I15">
         <v>1</v>
@@ -14584,7 +14655,7 @@
         <v>1</v>
       </c>
       <c r="H16">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="I16">
         <v>1</v>
@@ -14634,7 +14705,7 @@
         <v>1</v>
       </c>
       <c r="H17">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="I17">
         <v>1</v>
@@ -14684,7 +14755,7 @@
         <v>1</v>
       </c>
       <c r="H18">
-        <v>0.04</v>
+        <v>0.3</v>
       </c>
       <c r="I18">
         <v>1</v>
@@ -50656,8 +50727,8 @@
   <dimension ref="A1:N50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L38" sqref="L38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -50729,7 +50800,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>0.04</v>
+        <v>0.3</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -50773,7 +50844,7 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -50817,7 +50888,7 @@
         <v>1</v>
       </c>
       <c r="H4">
-        <v>0.04</v>
+        <v>0.3</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -50861,7 +50932,7 @@
         <v>1</v>
       </c>
       <c r="H5">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="I5">
         <v>1</v>
@@ -50905,7 +50976,7 @@
         <v>1</v>
       </c>
       <c r="H6">
-        <v>0.04</v>
+        <v>0.3</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -50949,7 +51020,7 @@
         <v>1</v>
       </c>
       <c r="H7">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="I7">
         <v>1</v>
@@ -50993,7 +51064,7 @@
         <v>1</v>
       </c>
       <c r="H8">
-        <v>0.04</v>
+        <v>0.3</v>
       </c>
       <c r="I8">
         <v>1</v>
@@ -51037,7 +51108,7 @@
         <v>1</v>
       </c>
       <c r="H9">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="I9">
         <v>1</v>
@@ -51081,7 +51152,7 @@
         <v>1</v>
       </c>
       <c r="H10">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="I10">
         <v>1</v>
@@ -51125,7 +51196,7 @@
         <v>1</v>
       </c>
       <c r="H11">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="I11">
         <v>1</v>
@@ -51169,7 +51240,7 @@
         <v>1</v>
       </c>
       <c r="H12">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="I12">
         <v>1</v>
@@ -51213,7 +51284,7 @@
         <v>1</v>
       </c>
       <c r="H13">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="I13">
         <v>1</v>
@@ -51257,7 +51328,7 @@
         <v>1</v>
       </c>
       <c r="H14">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="I14">
         <v>1</v>
@@ -51301,7 +51372,7 @@
         <v>1</v>
       </c>
       <c r="H15">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="I15">
         <v>1</v>
@@ -51345,7 +51416,7 @@
         <v>1</v>
       </c>
       <c r="H16">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="I16">
         <v>1</v>
@@ -51389,7 +51460,7 @@
         <v>1</v>
       </c>
       <c r="H17">
-        <v>0.04</v>
+        <v>0.3</v>
       </c>
       <c r="I17">
         <v>1</v>
@@ -51433,7 +51504,7 @@
         <v>1</v>
       </c>
       <c r="H18">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="I18">
         <v>1</v>
@@ -51477,7 +51548,7 @@
         <v>1</v>
       </c>
       <c r="H19">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="I19">
         <v>1</v>
@@ -51521,7 +51592,7 @@
         <v>1</v>
       </c>
       <c r="H20">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="I20">
         <v>1</v>
@@ -51565,7 +51636,7 @@
         <v>1</v>
       </c>
       <c r="H21">
-        <v>0.04</v>
+        <v>0.3</v>
       </c>
       <c r="I21">
         <v>1</v>
@@ -51609,7 +51680,7 @@
         <v>1</v>
       </c>
       <c r="H22">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="I22">
         <v>1</v>
@@ -51653,7 +51724,7 @@
         <v>1</v>
       </c>
       <c r="H23">
-        <v>0.04</v>
+        <v>0.3</v>
       </c>
       <c r="I23">
         <v>1</v>
@@ -51697,7 +51768,7 @@
         <v>1</v>
       </c>
       <c r="H24">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="I24">
         <v>1</v>
@@ -51741,7 +51812,7 @@
         <v>1</v>
       </c>
       <c r="H25">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="I25">
         <v>1</v>
@@ -51785,7 +51856,7 @@
         <v>1</v>
       </c>
       <c r="H26">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="I26">
         <v>1</v>
@@ -51829,7 +51900,7 @@
         <v>1</v>
       </c>
       <c r="H27">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="I27">
         <v>1</v>
@@ -51873,7 +51944,7 @@
         <v>1</v>
       </c>
       <c r="H28">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="I28">
         <v>1</v>
@@ -51917,7 +51988,7 @@
         <v>1</v>
       </c>
       <c r="H29">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="I29">
         <v>1</v>
@@ -51961,7 +52032,7 @@
         <v>1</v>
       </c>
       <c r="H30">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="I30">
         <v>1</v>
@@ -52005,7 +52076,7 @@
         <v>1</v>
       </c>
       <c r="H31">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="I31">
         <v>1</v>
@@ -52049,7 +52120,7 @@
         <v>1</v>
       </c>
       <c r="H32">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="I32">
         <v>1</v>
@@ -52093,7 +52164,7 @@
         <v>1</v>
       </c>
       <c r="H33">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="I33">
         <v>1</v>
@@ -52137,7 +52208,7 @@
         <v>1</v>
       </c>
       <c r="H34">
-        <v>0.04</v>
+        <v>0.3</v>
       </c>
       <c r="I34">
         <v>1</v>
@@ -52181,7 +52252,7 @@
         <v>1</v>
       </c>
       <c r="H35">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="I35">
         <v>1</v>
@@ -52225,7 +52296,7 @@
         <v>1</v>
       </c>
       <c r="H36">
-        <v>0.04</v>
+        <v>0.3</v>
       </c>
       <c r="I36">
         <v>1</v>
@@ -52269,7 +52340,7 @@
         <v>1</v>
       </c>
       <c r="H37">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="I37">
         <v>1</v>
@@ -52313,7 +52384,7 @@
         <v>1</v>
       </c>
       <c r="H38">
-        <v>0.04</v>
+        <v>0.3</v>
       </c>
       <c r="I38">
         <v>1</v>
@@ -52357,7 +52428,7 @@
         <v>1</v>
       </c>
       <c r="H39">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="I39">
         <v>1</v>
@@ -52401,7 +52472,7 @@
         <v>1</v>
       </c>
       <c r="H40">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="I40">
         <v>1</v>
@@ -52445,7 +52516,7 @@
         <v>1</v>
       </c>
       <c r="H41">
-        <v>0.04</v>
+        <v>0.3</v>
       </c>
       <c r="I41">
         <v>1</v>
@@ -52489,7 +52560,7 @@
         <v>1</v>
       </c>
       <c r="H42">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="I42">
         <v>1</v>
@@ -52533,7 +52604,7 @@
         <v>1</v>
       </c>
       <c r="H43">
-        <v>0.04</v>
+        <v>0.3</v>
       </c>
       <c r="I43">
         <v>1</v>
@@ -52577,7 +52648,7 @@
         <v>1</v>
       </c>
       <c r="H44">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="I44">
         <v>1</v>
@@ -52621,7 +52692,7 @@
         <v>1</v>
       </c>
       <c r="H45">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="I45">
         <v>1</v>
@@ -52665,7 +52736,7 @@
         <v>1</v>
       </c>
       <c r="H46">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="I46">
         <v>1</v>
@@ -52709,7 +52780,7 @@
         <v>1</v>
       </c>
       <c r="H47">
-        <v>0.04</v>
+        <v>0.3</v>
       </c>
       <c r="I47">
         <v>1</v>
@@ -52753,7 +52824,7 @@
         <v>1</v>
       </c>
       <c r="H48">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="I48">
         <v>1</v>
@@ -52797,7 +52868,7 @@
         <v>1</v>
       </c>
       <c r="H49">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="I49">
         <v>1</v>
@@ -52841,7 +52912,7 @@
         <v>1</v>
       </c>
       <c r="H50">
-        <v>0.04</v>
+        <v>0.3</v>
       </c>
       <c r="I50">
         <v>1</v>

</xml_diff>

<commit_message>
Update IL200 dynamic caes file and rerun case study
</commit_message>
<xml_diff>
--- a/ACTIVSg200/IL200_dyn_nl.xlsx
+++ b/ACTIVSg200/IL200_dyn_nl.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/work/turbinegov/ACTIVSg200/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE5535D-DCB8-684F-AD05-A34C3E246641}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B2DAB5-18B2-C44B-A154-B0BDE62A39CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1540" windowWidth="34560" windowHeight="19000" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="1540" windowWidth="34560" windowHeight="19000" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="2" r:id="rId1"/>
@@ -12308,9 +12308,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:AC18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AB12" sqref="AB12"/>
+      <selection pane="bottomLeft" activeCell="Z28" sqref="Z28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12487,7 +12487,7 @@
         <v>0</v>
       </c>
       <c r="AC2">
-        <v>5.0000000000000001E-3</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.2">
@@ -12573,7 +12573,7 @@
         <v>0</v>
       </c>
       <c r="AC3">
-        <v>5.0000000000000001E-3</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.2">
@@ -12659,7 +12659,7 @@
         <v>0</v>
       </c>
       <c r="AC4">
-        <v>5.0000000000000001E-3</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.2">
@@ -12745,7 +12745,7 @@
         <v>0</v>
       </c>
       <c r="AC5">
-        <v>5.0000000000000001E-3</v>
+        <v>200</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.2">
@@ -12831,7 +12831,7 @@
         <v>0</v>
       </c>
       <c r="AC6">
-        <v>5.0000000000000001E-3</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.2">
@@ -12917,7 +12917,7 @@
         <v>0</v>
       </c>
       <c r="AC7">
-        <v>5.0000000000000001E-3</v>
+        <v>200</v>
       </c>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.2">
@@ -13003,7 +13003,7 @@
         <v>0</v>
       </c>
       <c r="AC8">
-        <v>5.0000000000000001E-3</v>
+        <v>200</v>
       </c>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.2">
@@ -13089,7 +13089,7 @@
         <v>0</v>
       </c>
       <c r="AC9">
-        <v>5.0000000000000001E-3</v>
+        <v>200</v>
       </c>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.2">
@@ -13175,7 +13175,7 @@
         <v>0</v>
       </c>
       <c r="AC10">
-        <v>5.0000000000000001E-3</v>
+        <v>200</v>
       </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.2">
@@ -13261,7 +13261,7 @@
         <v>0</v>
       </c>
       <c r="AC11">
-        <v>5.0000000000000001E-3</v>
+        <v>200</v>
       </c>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.2">
@@ -13347,7 +13347,7 @@
         <v>0</v>
       </c>
       <c r="AC12">
-        <v>5.0000000000000001E-3</v>
+        <v>200</v>
       </c>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.2">
@@ -13433,7 +13433,7 @@
         <v>0</v>
       </c>
       <c r="AC13">
-        <v>5.0000000000000001E-3</v>
+        <v>200</v>
       </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.2">
@@ -13519,7 +13519,7 @@
         <v>0</v>
       </c>
       <c r="AC14">
-        <v>5.0000000000000001E-3</v>
+        <v>200</v>
       </c>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.2">
@@ -13605,7 +13605,7 @@
         <v>0</v>
       </c>
       <c r="AC15">
-        <v>5.0000000000000001E-3</v>
+        <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.2">
@@ -13691,7 +13691,7 @@
         <v>0</v>
       </c>
       <c r="AC16">
-        <v>5.0000000000000001E-3</v>
+        <v>200</v>
       </c>
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.2">
@@ -13777,7 +13777,7 @@
         <v>0</v>
       </c>
       <c r="AC17">
-        <v>5.0000000000000001E-3</v>
+        <v>200</v>
       </c>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.2">
@@ -13863,7 +13863,7 @@
         <v>0</v>
       </c>
       <c r="AC18">
-        <v>5.0000000000000001E-3</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -13875,7 +13875,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="O12" sqref="O12"/>
     </sheetView>

</xml_diff>